<commit_message>
Failed sprint4 adds (added before but for some reason it doesnt show)
</commit_message>
<xml_diff>
--- a/SE202526/Management/Sprint4/burndown/Sprint4_Burndown.xlsx
+++ b/SE202526/Management/Sprint4/burndown/Sprint4_Burndown.xlsx
@@ -12,14 +12,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="S6EO386pxAkXLUqJEEjy+6GzkG2xBoRkszmJrnTPxoY="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="TJwokC8WtZ8q3lTbP4pDtWS6JBud0zTpkznRah3M/MI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="77">
   <si>
     <t>Sprint 1 Burndown Chart</t>
   </si>
@@ -302,76 +302,7 @@
     </r>
   </si>
   <si>
-    <t>T19.1: Revisit the read code, and study the associated metrics.</t>
-  </si>
-  <si>
-    <t>T19.2: Revisit the read code, and study the associated metrics.</t>
-  </si>
-  <si>
-    <t>T19.3: Revisit the read code, and study the associated metrics.</t>
-  </si>
-  <si>
-    <t>T19.4: Revisit the read code, and study the associated metrics.</t>
-  </si>
-  <si>
-    <t>T19.5: Revisit the read code, and study the associated metrics.</t>
-  </si>
-  <si>
-    <t>T19.6: Revisit the read code, and study the associated metrics.</t>
-  </si>
-  <si>
-    <t>T20.1: Document said metrics.</t>
-  </si>
-  <si>
-    <t>T20.2: Document said metrics.</t>
-  </si>
-  <si>
-    <t>T20.3: Document said metrics.</t>
-  </si>
-  <si>
-    <t>T20.4: Document said metrics.</t>
-  </si>
-  <si>
-    <t>T20.5: Document said metrics.</t>
-  </si>
-  <si>
-    <t>T20.6: Document said metrics.</t>
-  </si>
-  <si>
-    <t>T21.1: Revisit the read code, and choose a part of the system to work on.</t>
-  </si>
-  <si>
-    <t>T21.2: Revisit the read code, and choose a part of the system to work on.</t>
-  </si>
-  <si>
-    <t>T21.3: Revisit the read code, and choose a part of the system to work on.</t>
-  </si>
-  <si>
-    <t>T21.4: Revisit the read code, and choose a part of the system to work on.</t>
-  </si>
-  <si>
-    <t>T21.5: Revisit the read code, and choose a part of the system to work on.</t>
-  </si>
-  <si>
-    <t>T21.6: Revisit the read code, and choose a part of the system to work on.</t>
-  </si>
-  <si>
-    <t>T22.1: Develop the Use Case Diagram of the chosen system part.</t>
-  </si>
-  <si>
-    <t>T22.2: Develop the Use Case Diagram of the chosen system part.</t>
-  </si>
-  <si>
-    <t>T22.3: Develop the Use Case Diagram of the chosen system part.</t>
-  </si>
-  <si>
-    <t>T22.4: Develop the Use Case Diagram of the chosen system part.</t>
-  </si>
-  <si>
-    <t>T22.5: Develop the Use Case Diagram of the chosen system part.</t>
-  </si>
-  <si>
-    <t>T22.6: Develop the Use Case Diagram of the chosen system part.</t>
+    <t>$$</t>
   </si>
   <si>
     <r>
@@ -402,7 +333,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -446,8 +377,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,12 +444,6 @@
         <bgColor rgb="FFC5E0B3"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="41">
     <border/>
@@ -952,7 +882,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="70">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1136,53 +1066,8 @@
     <xf borderId="12" fillId="3" fontId="4" numFmtId="15" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="22" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="21" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="24" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="39" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="34" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="38" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="34" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="40" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="34" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="34" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="40" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="33" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="40" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1295,8 +1180,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1974898631"/>
-        <c:axId val="827404185"/>
+        <c:axId val="1067990533"/>
+        <c:axId val="318874718"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1364,11 +1249,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1974898631"/>
-        <c:axId val="827404185"/>
+        <c:axId val="1067990533"/>
+        <c:axId val="318874718"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1974898631"/>
+        <c:axId val="1067990533"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,10 +1305,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="827404185"/>
+        <c:crossAx val="318874718"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="827404185"/>
+        <c:axId val="318874718"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15.0"/>
@@ -1488,7 +1373,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1974898631"/>
+        <c:crossAx val="1067990533"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1576,8 +1461,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="577046971"/>
-        <c:axId val="1262276433"/>
+        <c:axId val="463144813"/>
+        <c:axId val="110752417"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1645,11 +1530,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="577046971"/>
-        <c:axId val="1262276433"/>
+        <c:axId val="463144813"/>
+        <c:axId val="110752417"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="577046971"/>
+        <c:axId val="463144813"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,10 +1586,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1262276433"/>
+        <c:crossAx val="110752417"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1262276433"/>
+        <c:axId val="110752417"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15.0"/>
@@ -1769,7 +1654,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="577046971"/>
+        <c:crossAx val="463144813"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1857,8 +1742,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1833272964"/>
-        <c:axId val="984899137"/>
+        <c:axId val="1464094762"/>
+        <c:axId val="1165773373"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1926,11 +1811,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1833272964"/>
-        <c:axId val="984899137"/>
+        <c:axId val="1464094762"/>
+        <c:axId val="1165773373"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1833272964"/>
+        <c:axId val="1464094762"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1982,10 +1867,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="984899137"/>
+        <c:crossAx val="1165773373"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="984899137"/>
+        <c:axId val="1165773373"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16.0"/>
@@ -2050,7 +1935,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1833272964"/>
+        <c:crossAx val="1464094762"/>
         <c:majorUnit val="4.0"/>
         <c:minorUnit val="1.3333333333333333"/>
       </c:valAx>
@@ -2134,14 +2019,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint4'!$D$51:$K$51</c:f>
+              <c:f>'Burndown Chart Sprint4'!$D$26:$K$26</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1223306910"/>
-        <c:axId val="1930570348"/>
+        <c:axId val="205809955"/>
+        <c:axId val="953123066"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -2175,7 +2060,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint4'!$D$52:$K$52</c:f>
+              <c:f>'Burndown Chart Sprint4'!$D$27:$K$27</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2203,17 +2088,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint4'!$D$53:$K$53</c:f>
+              <c:f>'Burndown Chart Sprint4'!$D$28:$K$28</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1223306910"/>
-        <c:axId val="1930570348"/>
+        <c:axId val="205809955"/>
+        <c:axId val="953123066"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1223306910"/>
+        <c:axId val="205809955"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2265,10 +2150,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1930570348"/>
+        <c:crossAx val="953123066"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1930570348"/>
+        <c:axId val="953123066"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16.0"/>
@@ -2333,7 +2218,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1223306910"/>
+        <c:crossAx val="205809955"/>
         <c:majorUnit val="4.0"/>
         <c:minorUnit val="1.3333333333333333"/>
       </c:valAx>
@@ -2373,7 +2258,7 @@
     <xdr:ext cx="9639300" cy="4886325"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="418258697" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="545194366" name="Chart 1" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2403,7 +2288,7 @@
     <xdr:ext cx="9639300" cy="4886325"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3705767" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="231430725" name="Chart 2" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2433,7 +2318,7 @@
     <xdr:ext cx="9639300" cy="4886325"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1443805072" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="722181475" name="Chart 3" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2457,13 +2342,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9639300" cy="4886325"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1315158738" name="Chart 4" title="Chart"/>
+        <xdr:cNvPr id="1688031270" name="Chart 4" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5805,15 +5690,15 @@
         <v>0.1</v>
       </c>
       <c r="K8" s="31">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="L8" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>NOT ENOUGH WORK YET</v>
+        <v>DONE</v>
       </c>
       <c r="N8" s="60">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="O8" s="60" t="s">
         <v>41</v>
@@ -5976,10 +5861,10 @@
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="31">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="G13" s="31">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="H13" s="31"/>
       <c r="I13" s="32"/>
@@ -5987,11 +5872,11 @@
       <c r="K13" s="31"/>
       <c r="L13" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>NOT ENOUGH WORK YET</v>
+        <v>DONE</v>
       </c>
       <c r="N13" s="60">
         <f t="shared" si="2"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="O13" s="60" t="s">
         <v>49</v>
@@ -6858,11 +6743,11 @@
       </c>
       <c r="F38" s="39">
         <f t="shared" si="3"/>
-        <v>1.3</v>
+        <v>1.35</v>
       </c>
       <c r="G38" s="39">
         <f t="shared" si="3"/>
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="H38" s="39">
         <f t="shared" si="3"/>
@@ -6878,7 +6763,7 @@
       </c>
       <c r="K38" s="39">
         <f t="shared" si="3"/>
-        <v>2.35</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
@@ -6896,27 +6781,27 @@
       </c>
       <c r="F39" s="47">
         <f t="shared" si="4"/>
-        <v>13.7</v>
+        <v>13.65</v>
       </c>
       <c r="G39" s="47">
         <f t="shared" si="4"/>
-        <v>13.4</v>
+        <v>13.3</v>
       </c>
       <c r="H39" s="47">
         <f t="shared" si="4"/>
-        <v>12.7</v>
+        <v>12.6</v>
       </c>
       <c r="I39" s="48">
         <f t="shared" si="4"/>
-        <v>11.65</v>
+        <v>11.55</v>
       </c>
       <c r="J39" s="49">
         <f t="shared" si="4"/>
-        <v>8.85</v>
+        <v>8.75</v>
       </c>
       <c r="K39" s="49">
         <f t="shared" si="4"/>
-        <v>6.5</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
@@ -8056,25 +7941,25 @@
         <v>4</v>
       </c>
       <c r="E4" s="68">
-        <v>45963.0</v>
+        <v>45964.0</v>
       </c>
       <c r="F4" s="68">
-        <v>45964.0</v>
+        <v>45965.0</v>
       </c>
       <c r="G4" s="68">
-        <v>45965.0</v>
+        <v>45966.0</v>
       </c>
       <c r="H4" s="68">
-        <v>45966.0</v>
+        <v>45967.0</v>
       </c>
       <c r="I4" s="68">
-        <v>45967.0</v>
+        <v>45968.0</v>
       </c>
       <c r="J4" s="68">
-        <v>45968.0</v>
+        <v>45969.0</v>
       </c>
       <c r="K4" s="68">
-        <v>45969.0</v>
+        <v>45970.0</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -8106,17 +7991,20 @@
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="69" t="s">
+        <v>75</v>
+      </c>
       <c r="B6" s="28">
-        <v>14.1</v>
+        <v>11.0</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="69">
-        <v>0.05</v>
-      </c>
-      <c r="E6" s="70">
-        <v>0.05</v>
+        <v>38</v>
+      </c>
+      <c r="D6" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0.25</v>
       </c>
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
@@ -8125,18 +8013,18 @@
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
       <c r="L6" s="60" t="str">
-        <f t="shared" ref="L6:L50" si="1">IF(N6=0, "NOT STARTED" ,IF(N6&gt;D6, "ERROR TO MUCH WORK", IF(N6=D6, "DONE", "NOT ENOUGH WORK YET")))</f>
-        <v>DONE</v>
+        <f t="shared" ref="L6:L25" si="1">IF(N6=0, "NOT STARTED" ,IF(N6&gt;D6, "ERROR TO MUCH WORK", IF(N6=D6, "DONE", "NOT ENOUGH WORK YET")))</f>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N6" s="60">
-        <f t="shared" ref="N6:N50" si="2">SUM(E6:K6)</f>
-        <v>0.05</v>
+        <f t="shared" ref="N6:N25" si="2">SUM(E6:K6)</f>
+        <v>0.25</v>
       </c>
       <c r="O6" s="60" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P6" s="60">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
@@ -8146,21 +8034,21 @@
       <c r="C7" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="71">
-        <v>0.25</v>
-      </c>
-      <c r="E7" s="70">
-        <v>0.25</v>
-      </c>
+      <c r="D7" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="34"/>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
       <c r="I7" s="32"/>
-      <c r="J7" s="31"/>
+      <c r="J7" s="31">
+        <v>0.25</v>
+      </c>
       <c r="K7" s="31"/>
       <c r="L7" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N7" s="60">
         <f t="shared" si="2"/>
@@ -8175,67 +8063,69 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="B8" s="28">
-        <v>14.6</v>
-      </c>
-      <c r="C8" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="E8" s="70">
-        <v>0.1</v>
-      </c>
+        <v>15.1</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="34"/>
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="32"/>
       <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
+      <c r="K8" s="31">
+        <v>0.2</v>
+      </c>
       <c r="L8" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N8" s="60">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="O8" s="60" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="P8" s="60">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="B9" s="28">
-        <v>15.1</v>
+        <v>15.2</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="69">
-        <v>0.3</v>
-      </c>
-      <c r="E9" s="70">
-        <v>0.3</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="34"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="32"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
+      <c r="J9" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="K9" s="31">
+        <v>0.2</v>
+      </c>
       <c r="L9" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N9" s="60">
         <f t="shared" si="2"/>
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="O9" s="60" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P9" s="60">
         <v>15.0</v>
@@ -8243,33 +8133,35 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="B10" s="28">
-        <v>15.2</v>
+        <v>15.3</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="71">
-        <v>0.05</v>
-      </c>
-      <c r="E10" s="70">
-        <v>0.05</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="34"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="31"/>
+      <c r="I10" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="J10" s="31">
+        <v>0.3</v>
+      </c>
       <c r="K10" s="31"/>
       <c r="L10" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N10" s="60">
         <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="O10" s="60" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="P10" s="60">
         <v>15.0</v>
@@ -8277,33 +8169,35 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="B11" s="28">
-        <v>15.3</v>
+        <v>15.4</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="69">
-        <v>0.2</v>
-      </c>
-      <c r="E11" s="70">
-        <v>0.2</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="34"/>
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="31">
+        <v>0.2</v>
+      </c>
       <c r="I11" s="32"/>
       <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
+      <c r="K11" s="31">
+        <v>0.2</v>
+      </c>
       <c r="L11" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N11" s="60">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="O11" s="60" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="P11" s="60">
         <v>15.0</v>
@@ -8311,17 +8205,15 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="B12" s="28">
-        <v>15.4</v>
+        <v>15.5</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="69">
-        <v>0.4</v>
-      </c>
-      <c r="E12" s="70">
-        <v>0.4</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D12" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="34"/>
       <c r="F12" s="31"/>
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
@@ -8330,14 +8222,14 @@
       <c r="K12" s="31"/>
       <c r="L12" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT STARTED</v>
       </c>
       <c r="N12" s="60">
         <f t="shared" si="2"/>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="O12" s="60" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="P12" s="60">
         <v>15.0</v>
@@ -8345,35 +8237,35 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="B13" s="28">
-        <v>15.5</v>
+        <v>15.6</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="23">
+        <v>55</v>
+      </c>
+      <c r="D13" s="29">
         <v>0.5</v>
       </c>
-      <c r="E13" s="70">
-        <v>0.15</v>
-      </c>
-      <c r="F13" s="72">
-        <v>0.35</v>
-      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="32"/>
+      <c r="H13" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="I13" s="32">
+        <v>0.1</v>
+      </c>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N13" s="60">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="O13" s="60" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P13" s="60">
         <v>15.0</v>
@@ -8381,69 +8273,65 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="B14" s="28">
-        <v>15.6</v>
-      </c>
-      <c r="C14" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="69">
-        <v>0.15</v>
-      </c>
-      <c r="E14" s="70">
-        <v>0.15</v>
-      </c>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+        <v>16.4</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
       <c r="H14" s="31"/>
       <c r="I14" s="32"/>
       <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
+      <c r="K14" s="31">
+        <v>0.25</v>
+      </c>
       <c r="L14" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N14" s="60">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="O14" s="60" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P14" s="60">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="B15" s="28">
-        <v>16.4</v>
+        <v>16.5</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="69">
-        <v>0.25</v>
-      </c>
-      <c r="E15" s="70">
-        <v>0.2</v>
-      </c>
-      <c r="F15" s="72">
-        <v>0.05</v>
-      </c>
-      <c r="G15" s="72"/>
+        <v>60</v>
+      </c>
+      <c r="D15" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
       <c r="H15" s="31"/>
       <c r="I15" s="32"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
       <c r="L15" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT STARTED</v>
       </c>
       <c r="N15" s="60">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="O15" s="60" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="P15" s="60">
         <v>16.0</v>
@@ -8451,39 +8339,33 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="B16" s="28">
-        <v>16.5</v>
+        <v>16.6</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="23">
+        <v>61</v>
+      </c>
+      <c r="D16" s="29">
         <v>0.5</v>
       </c>
-      <c r="E16" s="70">
-        <v>0.1</v>
-      </c>
-      <c r="F16" s="72">
-        <v>0.3</v>
-      </c>
-      <c r="G16" s="72">
-        <v>0.05</v>
-      </c>
-      <c r="H16" s="72">
-        <v>0.05</v>
-      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="32"/>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N16" s="60">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="O16" s="60" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P16" s="60">
         <v>16.0</v>
@@ -8491,56 +8373,50 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="B17" s="28">
-        <v>16.6</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="69">
-        <v>0.25</v>
-      </c>
-      <c r="E17" s="70">
-        <v>0.1</v>
-      </c>
-      <c r="F17" s="72">
-        <v>0.15</v>
-      </c>
+        <v>17.4</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
       <c r="I17" s="32"/>
       <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
+      <c r="K17" s="31">
+        <v>0.2</v>
+      </c>
       <c r="L17" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N17" s="60">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="O17" s="60" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="P17" s="60">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="B18" s="28">
-        <v>17.4</v>
+        <v>17.5</v>
       </c>
       <c r="C18" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="69">
-        <v>0.3</v>
-      </c>
-      <c r="E18" s="70">
-        <v>0.2</v>
-      </c>
-      <c r="F18" s="72">
-        <v>0.1</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D18" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
       <c r="I18" s="32"/>
@@ -8548,14 +8424,14 @@
       <c r="K18" s="31"/>
       <c r="L18" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT STARTED</v>
       </c>
       <c r="N18" s="60">
         <f t="shared" si="2"/>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="O18" s="60" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="P18" s="60">
         <v>17.0</v>
@@ -8563,39 +8439,33 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="B19" s="28">
-        <v>17.5</v>
+        <v>17.6</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="23">
+        <v>67</v>
+      </c>
+      <c r="D19" s="29">
         <v>0.5</v>
       </c>
-      <c r="E19" s="70">
-        <v>0.05</v>
-      </c>
-      <c r="F19" s="72">
-        <v>0.15</v>
-      </c>
-      <c r="G19" s="72">
+      <c r="E19" s="34"/>
+      <c r="F19" s="31">
         <v>0.25</v>
       </c>
-      <c r="H19" s="72">
-        <v>0.05</v>
-      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
       <c r="I19" s="32"/>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
       <c r="L19" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N19" s="60">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="O19" s="60" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P19" s="60">
         <v>17.0</v>
@@ -8603,125 +8473,121 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="B20" s="28">
-        <v>17.6</v>
-      </c>
-      <c r="C20" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="69">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="70">
-        <v>0.05</v>
-      </c>
-      <c r="F20" s="72">
-        <v>0.1</v>
-      </c>
-      <c r="G20" s="72">
-        <v>0.1</v>
-      </c>
+        <v>18.1</v>
+      </c>
+      <c r="C20" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
       <c r="H20" s="31"/>
       <c r="I20" s="32"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
+      <c r="J20" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="K20" s="31">
+        <v>0.15</v>
+      </c>
       <c r="L20" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N20" s="60">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="O20" s="60" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="P20" s="60">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="B21" s="28">
-        <v>18.1</v>
+      <c r="B21" s="63">
+        <v>18.2</v>
       </c>
       <c r="C21" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="70">
-        <v>0.05</v>
-      </c>
-      <c r="F21" s="72">
-        <v>0.05</v>
-      </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
+        <v>69</v>
+      </c>
+      <c r="D21" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="64"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="67">
+        <v>0.15</v>
+      </c>
+      <c r="K21" s="65">
+        <v>0.15</v>
+      </c>
       <c r="L21" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N21" s="60">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="O21" s="60" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P21" s="60">
         <v>18.0</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="B22" s="63">
-        <v>18.2</v>
+      <c r="B22" s="28">
+        <v>18.3</v>
       </c>
       <c r="C22" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="71">
-        <v>0.2</v>
-      </c>
-      <c r="E22" s="73">
-        <v>0.2</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D22" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="64"/>
       <c r="F22" s="65"/>
       <c r="G22" s="65"/>
       <c r="H22" s="65"/>
       <c r="I22" s="66"/>
       <c r="J22" s="67"/>
-      <c r="K22" s="65"/>
+      <c r="K22" s="65">
+        <v>0.4</v>
+      </c>
       <c r="L22" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N22" s="60">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="O22" s="60" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="P22" s="60">
         <v>18.0</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="B23" s="28">
-        <v>18.3</v>
+      <c r="B23" s="63">
+        <v>18.4</v>
       </c>
       <c r="C23" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="E23" s="73">
-        <v>0.1</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D23" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="64"/>
       <c r="F23" s="65"/>
       <c r="G23" s="65"/>
       <c r="H23" s="65"/>
@@ -8730,35 +8596,31 @@
       <c r="K23" s="65"/>
       <c r="L23" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT STARTED</v>
       </c>
       <c r="N23" s="60">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="60" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="P23" s="60">
         <v>18.0</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="B24" s="63">
-        <v>18.4</v>
+      <c r="B24" s="28">
+        <v>18.5</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="29">
+        <v>72</v>
+      </c>
+      <c r="D24" s="23">
         <v>0.5</v>
       </c>
-      <c r="E24" s="73">
-        <v>0.25</v>
-      </c>
-      <c r="F24" s="74">
-        <v>0.25</v>
-      </c>
+      <c r="E24" s="64"/>
+      <c r="F24" s="65"/>
       <c r="G24" s="65"/>
       <c r="H24" s="65"/>
       <c r="I24" s="66"/>
@@ -8766,1049 +8628,190 @@
       <c r="K24" s="65"/>
       <c r="L24" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT STARTED</v>
       </c>
       <c r="N24" s="60">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O24" s="60" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="P24" s="60">
         <v>18.0</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="B25" s="28">
-        <v>18.5</v>
+      <c r="B25" s="63">
+        <v>18.6</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="23">
+        <v>73</v>
+      </c>
+      <c r="D25" s="29">
         <v>0.5</v>
       </c>
-      <c r="E25" s="73">
-        <v>0.0</v>
-      </c>
-      <c r="F25" s="74">
-        <v>0.1</v>
-      </c>
-      <c r="G25" s="74">
-        <v>0.35</v>
-      </c>
-      <c r="H25" s="74">
-        <v>0.05</v>
-      </c>
-      <c r="I25" s="66"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="66">
+        <v>0.25</v>
+      </c>
       <c r="J25" s="67"/>
       <c r="K25" s="65"/>
       <c r="L25" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N25" s="60">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="O25" s="60" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P25" s="60">
         <v>18.0</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="B26" s="63">
-        <v>18.6</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="69">
+      <c r="B26" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37">
+        <v>0.0</v>
+      </c>
+      <c r="E26" s="38">
+        <f t="shared" ref="E26:K26" si="3">SUM(E6:E20)</f>
         <v>0.25</v>
       </c>
-      <c r="E26" s="73">
-        <v>0.1</v>
-      </c>
-      <c r="F26" s="74">
-        <v>0.05</v>
-      </c>
-      <c r="G26" s="74">
-        <v>0.1</v>
-      </c>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N26" s="60">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="O26" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="P26" s="60">
-        <v>18.0</v>
+      <c r="F26" s="39">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="39">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+      <c r="I26" s="40">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="J26" s="41">
+        <f t="shared" si="3"/>
+        <v>1.05</v>
+      </c>
+      <c r="K26" s="39">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="B27" s="75">
-        <v>19.1</v>
-      </c>
-      <c r="C27" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E27" s="64"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="K27" s="65"/>
-      <c r="L27" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N27" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O27" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="P27" s="76">
-        <v>19.0</v>
+      <c r="B27" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45">
+        <f>SUM(D6:D26)</f>
+        <v>10</v>
+      </c>
+      <c r="E27" s="46">
+        <f t="shared" ref="E27:K27" si="4">D27-SUM(E6:E20)</f>
+        <v>9.75</v>
+      </c>
+      <c r="F27" s="47">
+        <f t="shared" si="4"/>
+        <v>9.25</v>
+      </c>
+      <c r="G27" s="47">
+        <f t="shared" si="4"/>
+        <v>9.25</v>
+      </c>
+      <c r="H27" s="47">
+        <f t="shared" si="4"/>
+        <v>8.8</v>
+      </c>
+      <c r="I27" s="48">
+        <f t="shared" si="4"/>
+        <v>8.6</v>
+      </c>
+      <c r="J27" s="49">
+        <f t="shared" si="4"/>
+        <v>7.55</v>
+      </c>
+      <c r="K27" s="49">
+        <f t="shared" si="4"/>
+        <v>6.35</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="B28" s="75">
-        <v>19.2</v>
-      </c>
-      <c r="C28" s="76" t="s">
+      <c r="B28" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E28" s="64"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="79">
-        <v>0.25</v>
-      </c>
-      <c r="J28" s="78">
-        <v>0.25</v>
-      </c>
-      <c r="K28" s="65"/>
-      <c r="L28" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N28" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O28" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="P28" s="76">
-        <v>19.0</v>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54">
+        <v>15.6</v>
+      </c>
+      <c r="E28" s="55">
+        <f>$D$28-($D$28/7*1)</f>
+        <v>13.37142857</v>
+      </c>
+      <c r="F28" s="55">
+        <f>$D$28-($D$28/7*2)</f>
+        <v>11.14285714</v>
+      </c>
+      <c r="G28" s="55">
+        <f>$D$28-($D$28/7*3)</f>
+        <v>8.914285714</v>
+      </c>
+      <c r="H28" s="55">
+        <f>$D$28-($D$28/7*4)</f>
+        <v>6.685714286</v>
+      </c>
+      <c r="I28" s="56">
+        <f>$D$28-($D$28/7*5)</f>
+        <v>4.457142857</v>
+      </c>
+      <c r="J28" s="56">
+        <f>$D$28-($D$28/7*6)</f>
+        <v>2.228571429</v>
+      </c>
+      <c r="K28" s="55">
+        <f>$D$28-($D$28/7*7)</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="B29" s="75">
-        <v>19.3</v>
-      </c>
-      <c r="C29" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E29" s="64"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="79">
-        <v>0.25</v>
-      </c>
-      <c r="J29" s="78">
-        <v>0.25</v>
-      </c>
-      <c r="K29" s="65"/>
-      <c r="L29" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N29" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O29" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="P29" s="76">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="B30" s="75">
-        <v>19.4</v>
-      </c>
-      <c r="C30" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E30" s="64"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="77"/>
-      <c r="J30" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="K30" s="65"/>
-      <c r="L30" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N30" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O30" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="P30" s="76">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="B31" s="75">
-        <v>19.5</v>
-      </c>
-      <c r="C31" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E31" s="64"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="K31" s="65"/>
-      <c r="L31" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N31" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O31" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="P31" s="76">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="B32" s="75">
-        <v>19.6</v>
-      </c>
-      <c r="C32" s="76" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E32" s="64"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="81">
-        <v>0.5</v>
-      </c>
-      <c r="K32" s="65"/>
-      <c r="L32" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N32" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O32" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="P32" s="76">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="B33" s="75">
-        <v>20.1</v>
-      </c>
-      <c r="C33" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E33" s="64"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="K33" s="65"/>
-      <c r="L33" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N33" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O33" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="P33" s="76">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="B34" s="75">
-        <v>20.2</v>
-      </c>
-      <c r="C34" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E34" s="64"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="K34" s="65"/>
-      <c r="L34" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N34" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O34" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="P34" s="76">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="B35" s="75">
-        <v>20.3</v>
-      </c>
-      <c r="C35" s="82" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E35" s="64"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="K35" s="65"/>
-      <c r="L35" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N35" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O35" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="P35" s="76">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="B36" s="75">
-        <v>20.4</v>
-      </c>
-      <c r="C36" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E36" s="64"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="K36" s="65"/>
-      <c r="L36" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N36" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O36" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="P36" s="76">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="B37" s="75">
-        <v>20.5</v>
-      </c>
-      <c r="C37" s="82" t="s">
-        <v>85</v>
-      </c>
-      <c r="D37" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E37" s="64"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="K37" s="65"/>
-      <c r="L37" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N37" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O37" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="P37" s="76">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="B38" s="75">
-        <v>20.6</v>
-      </c>
-      <c r="C38" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E38" s="64"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="66"/>
-      <c r="J38" s="83">
-        <v>0.5</v>
-      </c>
-      <c r="K38" s="65"/>
-      <c r="L38" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N38" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O38" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="P38" s="76">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="B39" s="75">
-        <v>21.1</v>
-      </c>
-      <c r="C39" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E39" s="64"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="74">
-        <v>0.5</v>
-      </c>
-      <c r="I39" s="66"/>
-      <c r="J39" s="67"/>
-      <c r="K39" s="65"/>
-      <c r="L39" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N39" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O39" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="P39" s="76">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="B40" s="75">
-        <v>21.2</v>
-      </c>
-      <c r="C40" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E40" s="64"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="74">
-        <v>0.25</v>
-      </c>
-      <c r="H40" s="74">
-        <v>0.25</v>
-      </c>
-      <c r="I40" s="66"/>
-      <c r="J40" s="67"/>
-      <c r="K40" s="65"/>
-      <c r="L40" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N40" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O40" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="P40" s="76">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="B41" s="75">
-        <v>21.3</v>
-      </c>
-      <c r="C41" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E41" s="64"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="74">
-        <v>0.25</v>
-      </c>
-      <c r="H41" s="74">
-        <v>0.25</v>
-      </c>
-      <c r="I41" s="66"/>
-      <c r="J41" s="67"/>
-      <c r="K41" s="65"/>
-      <c r="L41" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N41" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O41" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="P41" s="76">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="B42" s="75">
-        <v>21.4</v>
-      </c>
-      <c r="C42" s="76" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E42" s="64"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="74">
-        <v>0.5</v>
-      </c>
-      <c r="I42" s="66"/>
-      <c r="J42" s="67"/>
-      <c r="K42" s="65"/>
-      <c r="L42" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N42" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O42" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="P42" s="76">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="B43" s="75">
-        <v>21.5</v>
-      </c>
-      <c r="C43" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E43" s="64"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="74">
-        <v>0.5</v>
-      </c>
-      <c r="I43" s="66"/>
-      <c r="J43" s="67"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N43" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O43" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="P43" s="76">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="B44" s="75">
-        <v>21.6</v>
-      </c>
-      <c r="C44" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E44" s="64"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="74">
-        <v>0.5</v>
-      </c>
-      <c r="I44" s="66"/>
-      <c r="J44" s="67"/>
-      <c r="K44" s="65"/>
-      <c r="L44" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N44" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O44" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="P44" s="76">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="B45" s="75">
-        <v>22.1</v>
-      </c>
-      <c r="C45" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E45" s="64"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="74">
-        <v>0.15</v>
-      </c>
-      <c r="I45" s="84">
-        <v>0.25</v>
-      </c>
-      <c r="J45" s="83">
-        <v>0.1</v>
-      </c>
-      <c r="K45" s="65"/>
-      <c r="L45" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N45" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O45" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="P45" s="76">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="B46" s="75">
-        <v>22.2</v>
-      </c>
-      <c r="C46" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="D46" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E46" s="64"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="74">
-        <v>0.2</v>
-      </c>
-      <c r="H46" s="74">
-        <v>0.2</v>
-      </c>
-      <c r="I46" s="84">
-        <v>0.1</v>
-      </c>
-      <c r="J46" s="67"/>
-      <c r="K46" s="65"/>
-      <c r="L46" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N46" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O46" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="P46" s="76">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="B47" s="75">
-        <v>22.3</v>
-      </c>
-      <c r="C47" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="D47" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E47" s="64"/>
-      <c r="F47" s="74">
-        <v>0.0</v>
-      </c>
-      <c r="G47" s="74">
-        <v>0.2</v>
-      </c>
-      <c r="H47" s="74">
-        <v>0.3</v>
-      </c>
-      <c r="I47" s="66"/>
-      <c r="J47" s="67"/>
-      <c r="K47" s="65"/>
-      <c r="L47" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N47" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O47" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="P47" s="76">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="B48" s="75">
-        <v>22.4</v>
-      </c>
-      <c r="C48" s="82" t="s">
-        <v>96</v>
-      </c>
-      <c r="D48" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E48" s="64"/>
-      <c r="F48" s="65"/>
-      <c r="G48" s="65"/>
-      <c r="H48" s="74">
-        <v>0.1</v>
-      </c>
-      <c r="I48" s="84">
-        <v>0.4</v>
-      </c>
-      <c r="J48" s="67"/>
-      <c r="K48" s="65"/>
-      <c r="L48" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N48" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O48" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="P48" s="76">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="B49" s="75">
-        <v>22.5</v>
-      </c>
-      <c r="C49" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="64"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="65"/>
-      <c r="I49" s="84">
-        <v>0.25</v>
-      </c>
-      <c r="J49" s="83">
-        <v>0.25</v>
-      </c>
-      <c r="K49" s="65"/>
-      <c r="L49" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N49" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O49" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="P49" s="76">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="B50" s="75">
-        <v>22.6</v>
-      </c>
-      <c r="C50" s="82" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="E50" s="64"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="65"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="83">
-        <v>0.5</v>
-      </c>
-      <c r="K50" s="65"/>
-      <c r="L50" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE</v>
-      </c>
-      <c r="N50" s="60">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O50" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="P50" s="76">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="B51" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37">
-        <v>0.0</v>
-      </c>
-      <c r="E51" s="38">
-        <f t="shared" ref="E51:K51" si="3">SUM(E6:E21)</f>
-        <v>2.4</v>
-      </c>
-      <c r="F51" s="39">
-        <f t="shared" si="3"/>
-        <v>1.25</v>
-      </c>
-      <c r="G51" s="39">
-        <f t="shared" si="3"/>
-        <v>0.4</v>
-      </c>
-      <c r="H51" s="39">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="I51" s="40">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J51" s="41">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K51" s="39">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="B52" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="45">
-        <f>SUM(D6:D51)</f>
-        <v>17.7</v>
-      </c>
-      <c r="E52" s="46">
-        <f t="shared" ref="E52:K52" si="4">D52-SUM(E6:E21)</f>
-        <v>15.3</v>
-      </c>
-      <c r="F52" s="47">
-        <f t="shared" si="4"/>
-        <v>14.05</v>
-      </c>
-      <c r="G52" s="47">
-        <f t="shared" si="4"/>
-        <v>13.65</v>
-      </c>
-      <c r="H52" s="47">
-        <f t="shared" si="4"/>
-        <v>13.55</v>
-      </c>
-      <c r="I52" s="48">
-        <f t="shared" si="4"/>
-        <v>13.55</v>
-      </c>
-      <c r="J52" s="49">
-        <f t="shared" si="4"/>
-        <v>13.55</v>
-      </c>
-      <c r="K52" s="49">
-        <f t="shared" si="4"/>
-        <v>13.55</v>
-      </c>
-    </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="B53" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="53"/>
-      <c r="D53" s="54">
-        <v>15.6</v>
-      </c>
-      <c r="E53" s="55">
-        <f>$D$53-($D$53/7*1)</f>
-        <v>13.37142857</v>
-      </c>
-      <c r="F53" s="55">
-        <f>$D$53-($D$53/7*2)</f>
-        <v>11.14285714</v>
-      </c>
-      <c r="G53" s="55">
-        <f>$D$53-($D$53/7*3)</f>
-        <v>8.914285714</v>
-      </c>
-      <c r="H53" s="55">
-        <f>$D$53-($D$53/7*4)</f>
-        <v>6.685714286</v>
-      </c>
-      <c r="I53" s="56">
-        <f>$D$53-($D$53/7*5)</f>
-        <v>4.457142857</v>
-      </c>
-      <c r="J53" s="56">
-        <f>$D$53-($D$53/7*6)</f>
-        <v>2.228571429</v>
-      </c>
-      <c r="K53" s="55">
-        <f>$D$53-($D$53/7*7)</f>
-        <v>0</v>
-      </c>
-    </row>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
     <row r="54" ht="14.25" customHeight="1"/>
     <row r="55" ht="14.25" customHeight="1"/>
     <row r="56" ht="14.25" customHeight="1"/>
@@ -9984,31 +8987,31 @@
     <row r="226" ht="14.25" customHeight="1"/>
     <row r="227" ht="14.25" customHeight="1"/>
     <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
     <row r="254" ht="15.75" customHeight="1"/>
     <row r="255" ht="15.75" customHeight="1"/>
     <row r="256" ht="15.75" customHeight="1"/>
@@ -10744,51 +9747,8 @@
     <row r="986" ht="15.75" customHeight="1"/>
     <row r="987" ht="15.75" customHeight="1"/>
     <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
-    <row r="1009" ht="15.75" customHeight="1"/>
-    <row r="1010" ht="15.75" customHeight="1"/>
-    <row r="1011" ht="15.75" customHeight="1"/>
-    <row r="1012" ht="15.75" customHeight="1"/>
-    <row r="1013" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L48:M48"/>
+  <mergeCells count="27">
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="B4:B5"/>
@@ -10801,13 +9761,10 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="L12:M12"/>
     <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L20:M20"/>
@@ -10815,31 +9772,27 @@
     <mergeCell ref="L22:M22"/>
     <mergeCell ref="L23:M23"/>
     <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
   </mergeCells>
-  <conditionalFormatting sqref="L6:L50">
+  <conditionalFormatting sqref="L6:L25">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"DONE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:M50">
+  <conditionalFormatting sqref="L6:M25">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"NOT ENOUGH WORK YET"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:M50">
+  <conditionalFormatting sqref="L6:M25">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"ERROR TO MUCH WORK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6:N50">
+  <conditionalFormatting sqref="N7:N25">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -10851,7 +9804,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:M50">
+  <conditionalFormatting sqref="L6:M25">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"NOT STARTED"</formula>
     </cfRule>

</xml_diff>